<commit_message>
Modify Home Work Business Process Lesson9
</commit_message>
<xml_diff>
--- a/Process/Lesson9/BPLesson9.xlsx
+++ b/Process/Lesson9/BPLesson9.xlsx
@@ -11,9 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>Оцените 3 гипотезы по фреймворку RICE и выберите приоритетную</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>Оцените 5 гипотезы по фреймворку RICE и выберите приоритетную</t>
   </si>
   <si>
     <t xml:space="preserve">Оценка гипотез процесса  разработка программного модуля, кол-во пользователей 5000 </t>
@@ -23,13 +23,24 @@
 факторы</t>
   </si>
   <si>
-    <t>Качественное тестирование</t>
-  </si>
-  <si>
-    <t>Подготовка инфраструктуры</t>
-  </si>
-  <si>
-    <t>Подготовка персонала</t>
+    <t>Качественное
+планирование</t>
+  </si>
+  <si>
+    <t>Качественная 
+разработка</t>
+  </si>
+  <si>
+    <t>Качественное
+тестирование</t>
+  </si>
+  <si>
+    <t>Подготовка
+инфраструктуры</t>
+  </si>
+  <si>
+    <t>Подготовка
+персонала</t>
   </si>
   <si>
     <t>Reach</t>
@@ -47,7 +58,7 @@
     <t>Итого:</t>
   </si>
   <si>
-    <t>Посокльку с новой версией модуля будет работать только половина наших пользователей, на первое место выходит подготовка инфраструктуры, которая обеспечить корректную работу как старой так и новой версии модуля, второй на очереди стоит обучение персонала работе с нвовой версией и самый низкий приоритет имеет процесс тестирования в силу его высоких трудозотрат.</t>
+    <t>Посокльку с новой версией модуля будет работать только половина наших пользователей, на первое место выходит подготовка инфраструктуры, которая обеспечить корректную работу как старой так и новой версии модуля, второй на очереди стоит обучение персонала работе с нвовой версией и самый низкий приоритет имеет процесс разработки в силу его высоких трудозотрат.</t>
   </si>
   <si>
     <t>Предложите проект и просчитайте экономический эффект;</t>
@@ -56,7 +67,7 @@
     <t>Оценка дохода проекта разработки програмного модуля</t>
   </si>
   <si>
-    <t>Стстья</t>
+    <t>Статья</t>
   </si>
   <si>
     <t>1 год</t>
@@ -99,7 +110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -117,7 +128,6 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
-    <font/>
     <font>
       <sz val="11.0"/>
       <color rgb="FF2C2D30"/>
@@ -138,7 +148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border/>
     <border>
       <bottom style="thin">
@@ -149,14 +159,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -171,9 +173,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -198,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -218,42 +217,41 @@
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="3" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="3" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="3" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
@@ -481,27 +479,35 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="20.25"/>
-    <col customWidth="1" min="2" max="2" width="12.13"/>
-    <col customWidth="1" min="3" max="3" width="11.5"/>
-    <col customWidth="1" min="4" max="4" width="11.25"/>
-    <col customWidth="1" min="5" max="5" width="11.0"/>
-    <col customWidth="1" min="6" max="6" width="18.5"/>
+    <col customWidth="1" min="2" max="2" width="11.88"/>
+    <col customWidth="1" min="3" max="3" width="11.75"/>
+    <col customWidth="1" min="4" max="4" width="12.13"/>
+    <col customWidth="1" min="5" max="5" width="13.88"/>
+    <col customWidth="1" min="6" max="6" width="11.25"/>
+    <col customWidth="1" min="7" max="7" width="11.0"/>
+    <col customWidth="1" min="8" max="8" width="18.5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
@@ -510,260 +516,282 @@
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="F4" s="8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="10">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6">
+        <v>5000.0</v>
+      </c>
+      <c r="C5" s="10">
         <v>2500.0</v>
       </c>
-      <c r="C5" s="7"/>
       <c r="D5" s="10">
+        <v>2500.0</v>
+      </c>
+      <c r="E5" s="10">
         <v>5000.0</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="11">
+      <c r="F5" s="6">
         <v>2500.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="10">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="C6" s="10">
         <v>3.0</v>
       </c>
-      <c r="C6" s="7"/>
       <c r="D6" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="E6" s="10">
         <v>2.0</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="11">
+      <c r="F6" s="6">
         <v>3.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="10">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C7" s="10">
         <v>1.0</v>
       </c>
-      <c r="C7" s="7"/>
       <c r="D7" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="10">
         <v>0.8</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="11">
+      <c r="F7" s="6">
         <v>1.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="10">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6">
         <v>0.5</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="10">
+        <v>1.0</v>
+      </c>
       <c r="D8" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="10">
         <v>0.25</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="11">
+      <c r="F8" s="6">
         <v>0.25</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="13">
-        <f>(B5*B6*B7)/B8</f>
+      <c r="A9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="12">
+        <f t="shared" ref="B9:F9" si="1">(B5*B6*B7)/B8</f>
+        <v>16000</v>
+      </c>
+      <c r="C9" s="13">
+        <f t="shared" si="1"/>
+        <v>7500</v>
+      </c>
+      <c r="D9" s="13">
+        <f t="shared" si="1"/>
         <v>15000</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="13">
-        <f>(D5*D6*D7)/D8</f>
+      <c r="E9" s="13">
+        <f t="shared" si="1"/>
         <v>32000</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="14">
-        <f>(F5*F6*F7)/F8</f>
+      <c r="F9" s="12">
+        <f t="shared" si="1"/>
         <v>30000</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="15" t="s">
-        <v>11</v>
+      <c r="A11" s="14" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="16" t="s">
-        <v>12</v>
-      </c>
+      <c r="A13" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15">
-      <c r="A15" s="16" t="s">
-        <v>13</v>
-      </c>
+      <c r="A15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16">
-      <c r="A16" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="18" t="s">
+      <c r="A16" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="B16" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="C16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="D16" s="17" t="s">
         <v>19</v>
       </c>
+      <c r="E16" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="19">
+      <c r="A17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="18">
         <v>7500000.0</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
     </row>
     <row r="18">
-      <c r="A18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="19">
+      <c r="A18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="18">
         <v>3000000.0</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="18">
         <v>3500000.0</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="18">
         <v>4000000.0</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="18">
         <v>4100000.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="19">
+      <c r="A19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="18">
         <v>2500000.0</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="18">
         <v>1100000.0</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="18">
         <v>750000.0</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="18">
         <v>250000.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="14">
+      <c r="A20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="12">
         <f>-B17</f>
         <v>-7500000</v>
       </c>
-      <c r="C20" s="14">
-        <f t="shared" ref="C20:F20" si="1">C18-C19</f>
+      <c r="C20" s="12">
+        <f t="shared" ref="C20:F20" si="2">C18-C19</f>
         <v>500000</v>
       </c>
-      <c r="D20" s="14">
-        <f t="shared" si="1"/>
+      <c r="D20" s="12">
+        <f t="shared" si="2"/>
         <v>2400000</v>
       </c>
-      <c r="E20" s="14">
-        <f t="shared" si="1"/>
+      <c r="E20" s="12">
+        <f t="shared" si="2"/>
         <v>3250000</v>
       </c>
-      <c r="F20" s="14">
-        <f t="shared" si="1"/>
+      <c r="F20" s="12">
+        <f t="shared" si="2"/>
         <v>3850000</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="22">
+      <c r="A21" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="21">
         <v>0.1</v>
       </c>
-      <c r="E21" s="22"/>
+      <c r="G21" s="21"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="23">
-        <f>B20/(1+C21/100) + C20/POW(1+C21/100, 2) + D20/POW(1+C21/100, 3) + E20/POW(1+C21/100, 4) + F20/POW(1+C21/100, 5)</f>
+        <v>27</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22">
+        <f>B20/(1+E21/100) + C20/POW(1+E21/100, 2) + D20/POW(1+E21/100, 3) + E20/POW(1+E21/100, 4) + F20/POW(1+E21/100, 5)</f>
         <v>2467148.432</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="F23" s="24"/>
+      <c r="E23" s="22"/>
+      <c r="H23" s="23"/>
     </row>
     <row r="24">
-      <c r="A24" s="15" t="s">
-        <v>26</v>
+      <c r="A24" s="14" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="B9:C9"/>
+  <mergeCells count="7">
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A13:F13"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>